<commit_message>
Primer version funcional con GUI
Falta generar log para controlar hasta donde se mandaron los mails, y adjuntar un xlsx basico. Readme. Reemplazo de nombres y apellidos.
Error handling, selección de files opcional,
</commit_message>
<xml_diff>
--- a/Archivos adjuntos.xlsx
+++ b/Archivos adjuntos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Nexxos\Newsletter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Coding\Github\NEXXOS-emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3020C6FF-1D4D-442A-9D80-DF3F0F6A9354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7710EC-C4D4-479C-9ABD-5CAD3AC7A6E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Factura</t>
-  </si>
-  <si>
-    <t>Diploma</t>
-  </si>
-  <si>
     <t>Abbate</t>
   </si>
   <si>
@@ -51,12 +45,6 @@
     <t>abbatenicolas@gmail.com</t>
   </si>
   <si>
-    <t>abbate-f</t>
-  </si>
-  <si>
-    <t>abbate-d</t>
-  </si>
-  <si>
     <t>Capriata</t>
   </si>
   <si>
@@ -66,10 +54,22 @@
     <t>teficapriata@gmail.com</t>
   </si>
   <si>
-    <t>capriata-f</t>
-  </si>
-  <si>
-    <t>capriata-d</t>
+    <t>abbate-f.png</t>
+  </si>
+  <si>
+    <t>capriata-f.png</t>
+  </si>
+  <si>
+    <t>abbate-d.png</t>
+  </si>
+  <si>
+    <t>capriata-d.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas\Desktop\Coding\Github\NEXXOS-emails\Facturas</t>
+  </si>
+  <si>
+    <t>C:\Users\Lucas\Desktop\Coding\Github\NEXXOS-emails\Diplomas</t>
   </si>
 </sst>
 </file>
@@ -123,7 +123,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
@@ -131,13 +131,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 4" xfId="1" builtinId="19"/>
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -155,14 +167,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA9033D9-2570-4BDF-867E-383AF70758D1}" name="Tabla1" displayName="Tabla1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Encabezado 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA9033D9-2570-4BDF-867E-383AF70758D1}" name="Tabla1" displayName="Tabla1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Encabezado 4">
   <autoFilter ref="A1:E1048576" xr:uid="{A6575BCA-001B-4831-8F32-6F9A40192111}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4D3441E6-3D1A-4034-AD1C-D68B82A34C42}" name="Apellido"/>
     <tableColumn id="2" xr3:uid="{A73C9B1D-4DBA-427C-B3F9-59A94B1861DE}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{272F572F-2860-4E5A-A15A-2D396F8E12EE}" name="Mail"/>
-    <tableColumn id="4" xr3:uid="{E17568D9-DCE6-4C97-A259-19D7A1532254}" name="Factura"/>
-    <tableColumn id="5" xr3:uid="{93AD58CA-5431-40CD-AB80-09F417E507E0}" name="Diploma"/>
+    <tableColumn id="4" xr3:uid="{E17568D9-DCE6-4C97-A259-19D7A1532254}" name="C:\Users\Lucas\Desktop\Coding\Github\NEXXOS-emails\Facturas"/>
+    <tableColumn id="5" xr3:uid="{93AD58CA-5431-40CD-AB80-09F417E507E0}" name="C:\Users\Lucas\Desktop\Coding\Github\NEXXOS-emails\Diplomas" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,7 +446,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,11 +454,11 @@
     <col min="1" max="1" width="16.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" style="4" customWidth="1"/>
     <col min="3" max="3" width="24.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -457,48 +469,48 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E11" s="6"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="1"/>

</xml_diff>